<commit_message>
upgrade the App named excel
</commit_message>
<xml_diff>
--- a/src/main/java/org/codeman/core/personal/excel/test.xlsx
+++ b/src/main/java/org/codeman/core/personal/excel/test.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\win\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Z_relax\creative\src\main\java\org\codeman\core\personal\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3357589-53AD-4089-9B51-D3109FD70BFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53BD1BEC-BF02-4CA2-A482-78738DE79BED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1668" windowWidth="23040" windowHeight="10620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>A</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -35,11 +35,31 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>D</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>表头1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>表头2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>C</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>D</t>
+    <t>E</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>F</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>表头3</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -365,28 +385,45 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B2" t="s">
         <v>1</v>
       </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
-        <v>3</v>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>